<commit_message>
Modified name formatting in data files
</commit_message>
<xml_diff>
--- a/data/metaboliteData.xlsx
+++ b/data/metaboliteData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellaria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellaria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54367A2-C9DA-44D0-9CF1-980646E40FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A322D529-A4CF-441F-92D2-CB3E48906FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12540" yWindow="4680" windowWidth="15375" windowHeight="8325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="standards" sheetId="1" r:id="rId1"/>
@@ -624,10 +624,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9163,14 +9163,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -15374,8 +15374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91812B67-0FE2-4C51-BC0D-11966FFA1CC1}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:Q37"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17351,8 +17351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E826BF-5030-4592-B76A-B5EDD58F395B}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R43" sqref="R43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18365,161 +18365,161 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C20" s="7">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7">
-        <v>0</v>
-      </c>
-      <c r="H20" s="7">
-        <v>0</v>
-      </c>
-      <c r="I20" s="7">
-        <v>0</v>
-      </c>
-      <c r="J20" s="7">
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0</v>
+      </c>
+      <c r="J20" s="6">
         <v>0.65016470000000004</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="6">
         <v>0.27157924999999999</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="6">
         <v>73.231695599999995</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="6">
         <v>0.32333029000000002</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="6">
         <v>1.9924329700000001</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="6">
         <v>4.9640051200000004</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="6">
         <v>14.81007887</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q20" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>0.16464118999999999</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>0.49323623999999999</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>1.49511383</v>
       </c>
-      <c r="F21" s="7">
-        <v>0</v>
-      </c>
-      <c r="G21" s="7">
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
         <v>4.2063639999999999E-2</v>
       </c>
-      <c r="H21" s="7">
-        <v>0</v>
-      </c>
-      <c r="I21" s="7">
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6">
         <v>0.23228946</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="6">
         <v>0.1908337</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <v>7.7436039999999998E-2</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="6">
         <v>1.9525011999999999</v>
       </c>
-      <c r="M21" s="7">
-        <v>0</v>
-      </c>
-      <c r="N21" s="7">
-        <v>0</v>
-      </c>
-      <c r="O21" s="7">
+      <c r="M21" s="6">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0</v>
+      </c>
+      <c r="O21" s="6">
         <v>0.1599893</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P21" s="6">
         <v>5.43236E-2</v>
       </c>
-      <c r="Q21" s="7">
+      <c r="Q21" s="6">
         <v>2.9434869999999998E-2</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>0.26290350000000001</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>0.28460692999999998</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>0.39225459000000001</v>
       </c>
-      <c r="F22" s="7">
-        <v>0</v>
-      </c>
-      <c r="G22" s="7">
-        <v>0</v>
-      </c>
-      <c r="H22" s="7">
-        <v>0</v>
-      </c>
-      <c r="I22" s="7">
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6">
         <v>6.1539499170000003</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="6">
         <v>3.1100270999999999</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="6">
         <v>0.25310523000000001</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="6">
         <v>0.4404923</v>
       </c>
-      <c r="M22" s="7">
-        <v>0</v>
-      </c>
-      <c r="N22" s="7">
-        <v>0</v>
-      </c>
-      <c r="O22" s="7">
-        <v>0</v>
-      </c>
-      <c r="P22" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="7">
+      <c r="M22" s="6">
+        <v>0</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0</v>
+      </c>
+      <c r="O22" s="6">
+        <v>0</v>
+      </c>
+      <c r="P22" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>